<commit_message>
Finalizado o mapeamento das classes e executado a migration para o banco localDb
</commit_message>
<xml_diff>
--- a/Database/DadosIniciais.xlsx
+++ b/Database/DadosIniciais.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\GerenciadorEstoque\GerenciadorEstoque\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8317B1-2B7A-4F59-B7E2-5686C4D27965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CB0D39D2-1FD1-4764-BED0-9B0639E68037}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUTOS" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CATEGORIA!$B$1:$B$35</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,21 +39,21 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{A8FEC70B-A316-4B57-89FC-16589E1E61D1}" keepAlive="1" name="Consulta - cep" description="Conexão com a consulta 'cep' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Consulta - cep" description="Conexão com a consulta 'cep' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=cep;Extended Properties=&quot;&quot;" command="SELECT * FROM [cep]"/>
   </connection>
-  <connection id="2" xr16:uid="{A9F007AD-95C7-43BB-A6EF-D88C99223945}" keepAlive="1" name="Consulta - Enderecos" description="Conexão com a consulta 'Enderecos' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="2" keepAlive="1" name="Consulta - Enderecos" description="Conexão com a consulta 'Enderecos' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=Enderecos;Extended Properties=&quot;&quot;" command="SELECT * FROM [Enderecos]"/>
   </connection>
-  <connection id="3" xr16:uid="{3BB0A82F-28A0-4466-9D2F-983507C8436C}" keepAlive="1" name="Consulta - listPerson?qtdPessoas=6&amp;estado=10&amp;cidade=uberlandia&amp;gerarComPonto=true" description="Conexão com a consulta 'listPerson?qtdPessoas=6&amp;estado=10&amp;cidade=uberlandia&amp;gerarComPonto=true' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
+  <connection id="3" keepAlive="1" name="Consulta - listPerson?qtdPessoas=6&amp;estado=10&amp;cidade=uberlandia&amp;gerarComPonto=true" description="Conexão com a consulta 'listPerson?qtdPessoas=6&amp;estado=10&amp;cidade=uberlandia&amp;gerarComPonto=true' na pasta de trabalho." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;listPerson?qtdPessoas=6&amp;estado=10&amp;cidade=uberlandia&amp;gerarComPonto=true&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [listPerson?qtdPessoas=6&amp;estado=10&amp;cidade=uberlandia&amp;gerarComPonto=true]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="180">
   <si>
     <t>NOME</t>
   </si>
@@ -86,9 +85,6 @@
     <t>ENDERECO</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>DESCRIÇÃO</t>
   </si>
   <si>
@@ -314,12 +310,6 @@
     <t>'UN'</t>
   </si>
   <si>
-    <t>'18/03/2022'</t>
-  </si>
-  <si>
-    <t>18/03/2022'</t>
-  </si>
-  <si>
     <t>'APIARIOS MACKILANI LTDA'</t>
   </si>
   <si>
@@ -353,138 +343,6 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>Daniel Fonseca</t>
-  </si>
-  <si>
-    <t>Uberlândia</t>
-  </si>
-  <si>
-    <t>MG</t>
-  </si>
-  <si>
-    <t>Leandro Nelson Carlos da Costa</t>
-  </si>
-  <si>
-    <t>542.737.276-84</t>
-  </si>
-  <si>
-    <t>(34) 99845-8473</t>
-  </si>
-  <si>
-    <t>leandronelsoncarlosdacosta@mail.com</t>
-  </si>
-  <si>
-    <t>38400-670</t>
-  </si>
-  <si>
-    <t>Rua José Rezende dos Santos</t>
-  </si>
-  <si>
-    <t>Brasil</t>
-  </si>
-  <si>
-    <t>Rosa Yasmin Daiane</t>
-  </si>
-  <si>
-    <t>026.626.186-80</t>
-  </si>
-  <si>
-    <t>(34) 98715-9676</t>
-  </si>
-  <si>
-    <t>rosayasmindaiane@outlook.com</t>
-  </si>
-  <si>
-    <t>38421-046</t>
-  </si>
-  <si>
-    <t>Rua do Sai-Azul</t>
-  </si>
-  <si>
-    <t>Loteamento Residencial Pequis</t>
-  </si>
-  <si>
-    <t>Nina Jennifer Isabel</t>
-  </si>
-  <si>
-    <t>683.112.266-36</t>
-  </si>
-  <si>
-    <t>(34) 99813-3514</t>
-  </si>
-  <si>
-    <t>ninajenniferisabel@outlook.com</t>
-  </si>
-  <si>
-    <t>38421-643</t>
-  </si>
-  <si>
-    <t>Rua Odécio dos Santos</t>
-  </si>
-  <si>
-    <t>Residencial Lago Azul</t>
-  </si>
-  <si>
-    <t>Thomas Yago da Mota</t>
-  </si>
-  <si>
-    <t>741.781.786-60</t>
-  </si>
-  <si>
-    <t>(34) 98736-9088</t>
-  </si>
-  <si>
-    <t>thomasyagodamota@yahoo.com</t>
-  </si>
-  <si>
-    <t>38433-018</t>
-  </si>
-  <si>
-    <t>Rua Quatro</t>
-  </si>
-  <si>
-    <t>Vila Marielza</t>
-  </si>
-  <si>
-    <t>Danilo Severino Nathan Ribeiro</t>
-  </si>
-  <si>
-    <t>516.413.856-50</t>
-  </si>
-  <si>
-    <t>(34) 99779-7817</t>
-  </si>
-  <si>
-    <t>daniloseverinonathanribeiro@gmail.com</t>
-  </si>
-  <si>
-    <t>38400-708</t>
-  </si>
-  <si>
-    <t>Avenida Afonso Pena</t>
-  </si>
-  <si>
-    <t>Nossa Senhora Aparecida</t>
-  </si>
-  <si>
-    <t>Calebe Anderson Peixoto</t>
-  </si>
-  <si>
-    <t>846.236.776-05</t>
-  </si>
-  <si>
-    <t>(34) 99889-9582</t>
-  </si>
-  <si>
-    <t>calebeandersonpeixoto@hotmail.com</t>
-  </si>
-  <si>
-    <t>38400-329</t>
-  </si>
-  <si>
-    <t>Avenida Getúlio Vargas</t>
-  </si>
-  <si>
     <t>CEP</t>
   </si>
   <si>
@@ -503,58 +361,244 @@
     <t>NUMERO</t>
   </si>
   <si>
-    <t>32240-351</t>
-  </si>
-  <si>
-    <t>Beco Caramuru</t>
-  </si>
-  <si>
-    <t>Bandeirantes</t>
-  </si>
-  <si>
-    <t>Contagem</t>
-  </si>
-  <si>
-    <t>35302-660</t>
-  </si>
-  <si>
-    <t>Rua Marcelo Moreira Rezende de Araújo</t>
-  </si>
-  <si>
-    <t>Rafael José de Lima</t>
-  </si>
-  <si>
-    <t>Caratinga</t>
-  </si>
-  <si>
-    <t>38071-306</t>
-  </si>
-  <si>
-    <t>Avenida Doutor Milton Campos</t>
-  </si>
-  <si>
-    <t>Vila Arquelau</t>
-  </si>
-  <si>
-    <t>Uberaba</t>
-  </si>
-  <si>
-    <t>31540-474</t>
-  </si>
-  <si>
-    <t>Beco B</t>
-  </si>
-  <si>
-    <t>Jardim Leblon</t>
-  </si>
-  <si>
-    <t>Belo Horizonte</t>
+    <t>'38400-670'</t>
+  </si>
+  <si>
+    <t>'Rua José Rezende dos Santos'</t>
+  </si>
+  <si>
+    <t>'Brasil'</t>
+  </si>
+  <si>
+    <t>'Uberlândia'</t>
+  </si>
+  <si>
+    <t>'38421-046'</t>
+  </si>
+  <si>
+    <t>'Rua do Sai-Azul'</t>
+  </si>
+  <si>
+    <t>'Loteamento Residencial Pequis'</t>
+  </si>
+  <si>
+    <t>'38421-643'</t>
+  </si>
+  <si>
+    <t>'Rua Odécio dos Santos'</t>
+  </si>
+  <si>
+    <t>'Residencial Lago Azul'</t>
+  </si>
+  <si>
+    <t>'38433-018'</t>
+  </si>
+  <si>
+    <t>'Rua Quatro'</t>
+  </si>
+  <si>
+    <t>'Vila Marielza'</t>
+  </si>
+  <si>
+    <t>'38400-708'</t>
+  </si>
+  <si>
+    <t>'Avenida Afonso Pena'</t>
+  </si>
+  <si>
+    <t>'Nossa Senhora Aparecida'</t>
+  </si>
+  <si>
+    <t>'38400-329'</t>
+  </si>
+  <si>
+    <t>'Avenida Getúlio Vargas'</t>
+  </si>
+  <si>
+    <t>'Daniel Fonseca'</t>
+  </si>
+  <si>
+    <t>'32240-351'</t>
+  </si>
+  <si>
+    <t>'Beco Caramuru'</t>
+  </si>
+  <si>
+    <t>'Bandeirantes'</t>
+  </si>
+  <si>
+    <t>'Contagem'</t>
+  </si>
+  <si>
+    <t>'35302-660'</t>
+  </si>
+  <si>
+    <t>'Rua Marcelo Moreira Rezende de Araújo'</t>
+  </si>
+  <si>
+    <t>'Rafael José de Lima'</t>
+  </si>
+  <si>
+    <t>'Caratinga'</t>
+  </si>
+  <si>
+    <t>'38071-306'</t>
+  </si>
+  <si>
+    <t>'Avenida Doutor Milton Campos'</t>
+  </si>
+  <si>
+    <t>'Vila Arquelau'</t>
+  </si>
+  <si>
+    <t>'Uberaba'</t>
+  </si>
+  <si>
+    <t>'31540-474'</t>
+  </si>
+  <si>
+    <t>'Beco B'</t>
+  </si>
+  <si>
+    <t>'Jardim Leblon'</t>
+  </si>
+  <si>
+    <t>'Belo Horizonte'</t>
+  </si>
+  <si>
+    <t>'MG'</t>
+  </si>
+  <si>
+    <t>'Leandro Nelson Carlos da Costa'</t>
+  </si>
+  <si>
+    <t>'542.737.276-84'</t>
+  </si>
+  <si>
+    <t>'(34) 99845-8473'</t>
+  </si>
+  <si>
+    <t>'leandronelsoncarlosdacosta@mail.com'</t>
+  </si>
+  <si>
+    <t>'Rosa Yasmin Daiane'</t>
+  </si>
+  <si>
+    <t>'026.626.186-80'</t>
+  </si>
+  <si>
+    <t>'(34) 98715-9676'</t>
+  </si>
+  <si>
+    <t>'rosayasmindaiane@outlook.com'</t>
+  </si>
+  <si>
+    <t>'Nina Jennifer Isabel'</t>
+  </si>
+  <si>
+    <t>'683.112.266-36'</t>
+  </si>
+  <si>
+    <t>'(34) 99813-3514'</t>
+  </si>
+  <si>
+    <t>'ninajenniferisabel@outlook.com'</t>
+  </si>
+  <si>
+    <t>'Thomas Yago da Mota'</t>
+  </si>
+  <si>
+    <t>'741.781.786-60'</t>
+  </si>
+  <si>
+    <t>'(34) 98736-9088'</t>
+  </si>
+  <si>
+    <t>'thomasyagodamota@yahoo.com'</t>
+  </si>
+  <si>
+    <t>'Danilo Severino Nathan Ribeiro'</t>
+  </si>
+  <si>
+    <t>'516.413.856-50'</t>
+  </si>
+  <si>
+    <t>'(34) 99779-7817'</t>
+  </si>
+  <si>
+    <t>'daniloseverinonathanribeiro@gmail.com'</t>
+  </si>
+  <si>
+    <t>'Calebe Anderson Peixoto'</t>
+  </si>
+  <si>
+    <t>'846.236.776-05'</t>
+  </si>
+  <si>
+    <t>'(34) 99889-9582'</t>
+  </si>
+  <si>
+    <t>'calebeandersonpeixoto@hotmail.com'</t>
+  </si>
+  <si>
+    <t>'2022-03-01'</t>
+  </si>
+  <si>
+    <t>'2022-03-02'</t>
+  </si>
+  <si>
+    <t>'2022-03-03'</t>
+  </si>
+  <si>
+    <t>'2022-03-04'</t>
+  </si>
+  <si>
+    <t>'2022-03-05'</t>
+  </si>
+  <si>
+    <t>'2022-03-06'</t>
+  </si>
+  <si>
+    <t>'2022-03-08'</t>
+  </si>
+  <si>
+    <t>'2022-03-09'</t>
+  </si>
+  <si>
+    <t>'2022-03-10'</t>
+  </si>
+  <si>
+    <t>'2022-03-11'</t>
+  </si>
+  <si>
+    <t>'2022-03-12'</t>
+  </si>
+  <si>
+    <t>'2022-03-13'</t>
+  </si>
+  <si>
+    <t>'2022-03-14'</t>
+  </si>
+  <si>
+    <t>'2022-03-15'</t>
+  </si>
+  <si>
+    <t>'2022-03-16'</t>
+  </si>
+  <si>
+    <t>'2022-03-17'</t>
+  </si>
+  <si>
+    <t>'2022-03-18'</t>
+  </si>
+  <si>
+    <t>'2022-03-19'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -613,15 +657,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,11 +980,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEB1402-0448-4CD4-9A5E-49E2DF45B6C9}">
-  <dimension ref="A1:K35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +992,7 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
@@ -957,12 +1002,12 @@
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -983,1207 +1028,1484 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>44.328899999999997</v>
       </c>
       <c r="E2">
-        <f>D2-(D2*0.55)</f>
+        <f t="shared" ref="E2:E34" si="0">D2-(D2*0.55)</f>
         <v>19.948004999999998</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
-        <v>10</v>
+      <c r="H2">
+        <v>1</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>87</v>
+        <v>162</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="str">
+        <f>"INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;E2&amp;", "&amp;D2&amp;", "&amp;G2&amp;", "&amp;F2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;")"</f>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(1, '0000000000001', 'ABSOLUT PASTA AMENDOIM BEIJINHO 1KG', 19.948005, 44.3289, 9, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>33.218899999999998</v>
       </c>
       <c r="E3">
-        <f>D3-(D3*0.55)</f>
+        <f t="shared" si="0"/>
         <v>14.948504999999997</v>
       </c>
       <c r="F3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
-        <v>10</v>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="str">
+        <f t="shared" ref="L3:L34" si="1">"INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;E3&amp;", "&amp;D3&amp;", "&amp;G3&amp;", "&amp;F3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;")"</f>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(2, '0000000000002', 'ABSOLUT PASTA AMENDOIM BEIJINHO 500G', 14.948505, 33.2189, 8, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>44.328899999999997</v>
       </c>
       <c r="E4">
-        <f>D4-(D4*0.55)</f>
+        <f t="shared" si="0"/>
         <v>19.948004999999998</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
-        <v>10</v>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(3, '0000000000003', 'ABSOLUT PASTA AMENDOIM BROWNIE 1KG', 19.948005, 44.3289, 7, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>33.218899999999998</v>
       </c>
       <c r="E5">
-        <f>D5-(D5*0.55)</f>
+        <f t="shared" si="0"/>
         <v>14.948504999999997</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
-        <v>10</v>
+      <c r="H5">
+        <v>1</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(4, '0000000000004', 'ABSOLUT PASTA AMENDOIM BROWNIE 500G', 14.948505, 33.2189, 4, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>8.6102500000000006</v>
       </c>
       <c r="E6">
-        <f>D6-(D6*0.55)</f>
+        <f t="shared" si="0"/>
         <v>3.8746124999999996</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
-        <v>10</v>
+      <c r="H6">
+        <v>1</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>86</v>
+        <v>162</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(5, '0000000000005', 'ACAI BANANA ECO FLASH 200G', 3.8746125, 8.61025, 5, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7">
         <v>27.663899999999998</v>
       </c>
       <c r="E7">
-        <f>D7-(D7*0.55)</f>
+        <f t="shared" si="0"/>
         <v>12.448754999999998</v>
       </c>
       <c r="F7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
-        <v>10</v>
+      <c r="H7">
+        <v>1</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(6, '0000000000006', 'ACAI DESIDRATADO TIARAJU 150G', 12.448755, 27.6639, 6, 'UN', 1, '2022-03-02', '2022-03-02', 1)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8">
         <v>28.774899999999999</v>
       </c>
       <c r="E8">
-        <f>D8-(D8*0.55)</f>
+        <f t="shared" si="0"/>
         <v>12.948704999999999</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8">
         <v>4</v>
       </c>
-      <c r="H8" t="s">
-        <v>10</v>
+      <c r="H8">
+        <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(7, '0000000000007', 'ACAI ECO FLESH GUARANA 1000G', 12.948705, 28.7749, 4, 'UN', 1, '2022-03-02', '2022-03-02', 1)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>38.773899999999998</v>
       </c>
       <c r="E9">
-        <f>D9-(D9*0.55)</f>
+        <f t="shared" si="0"/>
         <v>17.448254999999996</v>
       </c>
       <c r="F9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9">
         <v>5</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
+      <c r="H9">
+        <v>1</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="K9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(8, '0000000000008', 'ADOCANTE ABSOLUT 100% ESTEVIA 150G', 17.448255, 38.7739, 5, 'UN', 1, '2022-03-03', '2022-03-03', 4)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>44.328899999999997</v>
       </c>
       <c r="E10">
-        <f>D10-(D10*0.55)</f>
+        <f t="shared" si="0"/>
         <v>19.948004999999998</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10">
         <v>8</v>
       </c>
-      <c r="H10" t="s">
-        <v>10</v>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
       <c r="K10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(9, '0000000000009', 'ADOCANTE ABSOLUT 100% XYLITOL 300G', 19.948005, 44.3289, 8, 'UN', 1, '2022-03-03', '2022-03-03', 4)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>18.220399999999998</v>
       </c>
       <c r="E11">
-        <f>D11-(D11*0.55)</f>
+        <f t="shared" si="0"/>
         <v>8.1991799999999984</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>9</v>
       </c>
-      <c r="H11" t="s">
-        <v>10</v>
+      <c r="H11">
+        <v>1</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="K11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(10, '0000000000010', 'ADOCANTE AIROM TAUMATINA 100 ML', 8.19918, 18.2204, 9, 'UN', 1, '2022-03-04', '2022-03-04', 4)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>59.882899999999999</v>
       </c>
       <c r="E12">
-        <f>D12-(D12*0.55)</f>
+        <f t="shared" si="0"/>
         <v>26.947305</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12">
         <v>6</v>
       </c>
-      <c r="H12" t="s">
-        <v>10</v>
+      <c r="H12">
+        <v>1</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="K12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(11, '0000000000011', 'ALBUMINA MILLENNIUM BAUNILHA 500G', 26.947305, 59.8829, 6, 'UN', 1, '2022-03-04', '2022-03-04', 2)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>59.882899999999999</v>
       </c>
       <c r="E13">
-        <f>D13-(D13*0.55)</f>
+        <f t="shared" si="0"/>
         <v>26.947305</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13">
         <v>8</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
+      <c r="H13">
+        <v>1</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="K13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(12, '0000000000012', 'ALBUMINA MILLENNIUM CHOCOLATE 500G', 26.947305, 59.8829, 8, 'UN', 1, '2022-03-04', '2022-03-04', 2)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>59.882899999999999</v>
       </c>
       <c r="E14">
-        <f>D14-(D14*0.55)</f>
+        <f t="shared" si="0"/>
         <v>26.947305</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14">
         <v>5</v>
       </c>
-      <c r="H14" t="s">
-        <v>10</v>
+      <c r="H14">
+        <v>1</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>86</v>
+        <v>166</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(13, '0000000000013', 'ALBUMINA MILLENNIUM MOR.BANANA.500G', 26.947305, 59.8829, 5, 'UN', 1, '2022-03-05', '2022-03-05', 2)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>12.7765</v>
       </c>
       <c r="E15">
-        <f>D15-(D15*0.55)</f>
+        <f t="shared" si="0"/>
         <v>5.7494249999999996</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15">
         <v>5</v>
       </c>
-      <c r="H15" t="s">
-        <v>10</v>
+      <c r="H15">
+        <v>1</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="K15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(14, '0000000000014', 'BANANINHA HUE 117G', 5.749425, 12.7765, 5, 'UN', 1, '2022-03-06', '2022-03-06', 2)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16">
         <v>14.331900000000001</v>
       </c>
       <c r="E16">
-        <f>D16-(D16*0.55)</f>
+        <f t="shared" si="0"/>
         <v>6.4493549999999997</v>
       </c>
       <c r="F16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16">
         <v>7</v>
       </c>
-      <c r="H16" t="s">
-        <v>10</v>
+      <c r="H16">
+        <v>1</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>86</v>
+        <v>167</v>
       </c>
       <c r="K16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(15, '0000000000015', 'BANANINHA NUTRYLLACK 28G', 6.449355, 14.3319, 7, 'UN', 1, '2022-03-06', '2022-03-06', 2)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17">
         <v>30.996899999999997</v>
       </c>
       <c r="E17">
-        <f>D17-(D17*0.55)</f>
+        <f t="shared" si="0"/>
         <v>13.948604999999997</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17">
         <v>4</v>
       </c>
-      <c r="H17" t="s">
-        <v>10</v>
+      <c r="H17">
+        <v>1</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="K17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(16, '0000000000016', 'BANANINHA PASSA TIPIKUS 1 KG', 13.948605, 30.9969, 4, 'UN', 1, '2022-03-08', '2022-03-08', 2)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D18">
         <v>115.4329</v>
       </c>
       <c r="E18">
-        <f>D18-(D18*0.55)</f>
+        <f t="shared" si="0"/>
         <v>51.944804999999995</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G18">
         <v>9</v>
       </c>
-      <c r="H18" t="s">
-        <v>10</v>
+      <c r="H18">
+        <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="K18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(17, '0000000000017', 'BCAA PLUS PROBIOTICA 120 CAP', 51.944805, 115.4329, 9, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19">
         <v>84.047150000000002</v>
       </c>
       <c r="E19">
-        <f>D19-(D19*0.55)</f>
+        <f t="shared" si="0"/>
         <v>37.821217499999996</v>
       </c>
       <c r="F19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G19">
         <v>5</v>
       </c>
-      <c r="H19" t="s">
-        <v>10</v>
+      <c r="H19">
+        <v>1</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="K19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(18, '0000000000018', 'BCAA PRO PROBIOTICA 120 CAP', 37.8212175, 84.04715, 5, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20">
         <v>38.773899999999998</v>
       </c>
       <c r="E20">
-        <f>D20-(D20*0.55)</f>
+        <f t="shared" si="0"/>
         <v>17.448254999999996</v>
       </c>
       <c r="F20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G20">
         <v>3</v>
       </c>
-      <c r="H20" t="s">
-        <v>10</v>
+      <c r="H20">
+        <v>1</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="K20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(19, '0000000000019', 'BCAA PRO PROBIOTICA 60 CAPS', 17.448255, 38.7739, 3, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21">
         <v>194.42500000000001</v>
       </c>
       <c r="E21">
-        <f>D21-(D21*0.55)</f>
+        <f t="shared" si="0"/>
         <v>87.491249999999994</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21">
         <v>8</v>
       </c>
-      <c r="H21" t="s">
-        <v>10</v>
+      <c r="H21">
+        <v>1</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="K21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(20, '0000000000020', 'BCAA PROBIOTICA BLACK NATURAL 300G', 87.49125, 194.425, 8, 'UN', 1, '2022-03-09', '2022-03-09', 2)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D22">
         <v>41.106999999999999</v>
       </c>
       <c r="E22">
-        <f>D22-(D22*0.55)</f>
+        <f t="shared" si="0"/>
         <v>18.498149999999999</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22">
         <v>9</v>
       </c>
-      <c r="H22" t="s">
-        <v>10</v>
+      <c r="H22">
+        <v>1</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="K22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(21, '0000000000021', 'CREATINA INTEGRAL 100G', 18.49815, 41.107, 9, 'UN', 1, '2022-03-10', '2022-03-10', 2)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23">
         <v>72.10390000000001</v>
       </c>
       <c r="E23">
-        <f>D23-(D23*0.55)</f>
+        <f t="shared" si="0"/>
         <v>32.446755000000003</v>
       </c>
       <c r="F23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G23">
         <v>9</v>
       </c>
-      <c r="H23" t="s">
-        <v>10</v>
+      <c r="H23">
+        <v>1</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="K23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(22, '0000000000022', 'CREATINA INTEGRAL 120 CAPS', 32.446755, 72.1039, 9, 'UN', 1, '2022-03-10', '2022-03-10', 3)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24">
         <v>92.768500000000003</v>
       </c>
       <c r="E24">
-        <f>D24-(D24*0.55)</f>
+        <f t="shared" si="0"/>
         <v>41.745824999999996</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G24">
         <v>3</v>
       </c>
-      <c r="H24" t="s">
-        <v>10</v>
+      <c r="H24">
+        <v>1</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>86</v>
+        <v>171</v>
       </c>
       <c r="K24">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(23, '0000000000023', 'CREATINA INTEGRAL 120 CPS', 41.745825, 92.7685, 3, 'UN', 1, '2022-03-11', '2022-03-11', 3)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25">
         <v>12.60985</v>
       </c>
       <c r="E25">
-        <f>D25-(D25*0.55)</f>
+        <f t="shared" si="0"/>
         <v>5.6744324999999991</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G25">
         <v>5</v>
       </c>
-      <c r="H25" t="s">
-        <v>10</v>
+      <c r="H25">
+        <v>1</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="K25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(24, '0000000000024', 'CRISTAIS GENGIBRE ARDRAK ANIS 22G', 5.6744325, 12.60985, 5, 'UN', 1, '2022-03-12', '2022-03-12', 4)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D26">
         <v>12.60985</v>
       </c>
       <c r="E26">
-        <f>D26-(D26*0.55)</f>
+        <f t="shared" si="0"/>
         <v>5.6744324999999991</v>
       </c>
       <c r="F26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26">
         <v>5</v>
       </c>
-      <c r="H26" t="s">
-        <v>10</v>
+      <c r="H26">
+        <v>1</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>86</v>
+        <v>173</v>
       </c>
       <c r="K26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(25, '0000000000025', 'CRISTAIS GENGIBRE ARDRAK CANELA 22G', 5.6744325, 12.60985, 5, 'UN', 1, '2022-03-13', '2022-03-13', 4)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27">
         <v>12.60985</v>
       </c>
       <c r="E27">
-        <f>D27-(D27*0.55)</f>
+        <f t="shared" si="0"/>
         <v>5.6744324999999991</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27">
         <v>7</v>
       </c>
-      <c r="H27" t="s">
-        <v>10</v>
+      <c r="H27">
+        <v>1</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="K27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(26, '0000000000026', 'CRISTAIS GENGIBRE ARDRAK FRU.CITRICAS 22G', 5.6744325, 12.60985, 7, 'UN', 1, '2022-03-14', '2022-03-14', 4)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28">
         <v>383.29500000000002</v>
       </c>
       <c r="E28">
-        <f>D28-(D28*0.55)</f>
+        <f t="shared" si="0"/>
         <v>172.48274999999998</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28">
         <v>7</v>
       </c>
-      <c r="H28" t="s">
-        <v>10</v>
+      <c r="H28">
+        <v>1</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="K28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(27, '0000000000027', 'ISO 100 WHEY DYMATIZE BAUNILHA 726G', 172.48275, 383.295, 7, 'UN', 1, '2022-03-14', '2022-03-14', 3)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D29">
         <v>383.29500000000002</v>
       </c>
       <c r="E29">
-        <f>D29-(D29*0.55)</f>
+        <f t="shared" si="0"/>
         <v>172.48274999999998</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29">
         <v>7</v>
       </c>
-      <c r="H29" t="s">
-        <v>10</v>
+      <c r="H29">
+        <v>1</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="K29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(28, '0000000000028', 'ISO 100 WHEY DYMATIZE BOLO ANIVERSARIO 726G', 172.48275, 383.295, 7, 'UN', 1, '2022-03-14', '2022-03-14', 3)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30">
         <v>398.84899999999999</v>
       </c>
       <c r="E30">
-        <f>D30-(D30*0.55)</f>
+        <f t="shared" si="0"/>
         <v>179.48204999999999</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G30">
         <v>4</v>
       </c>
-      <c r="H30" t="s">
-        <v>10</v>
+      <c r="H30">
+        <v>1</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="J30" s="5" t="s">
-        <v>86</v>
+        <v>175</v>
       </c>
       <c r="K30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(29, '0000000000029', 'ISO 100 WHEY DYMATIZE BROWNIE 893G', 179.48205, 398.849, 4, 'UN', 1, '2022-03-15', '2022-03-15', 3)</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D31">
         <v>398.84899999999999</v>
       </c>
       <c r="E31">
-        <f>D31-(D31*0.55)</f>
+        <f t="shared" si="0"/>
         <v>179.48204999999999</v>
       </c>
       <c r="F31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G31">
         <v>3</v>
       </c>
-      <c r="H31" t="s">
-        <v>10</v>
+      <c r="H31">
+        <v>1</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>86</v>
+        <v>176</v>
       </c>
       <c r="K31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(30, '0000000000030', 'ISO 100 WHEY DYMATIZE CAKE 893G', 179.48205, 398.849, 3, 'UN', 1, '2022-03-16', '2022-03-16', 3)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32">
         <v>16.553899999999999</v>
       </c>
       <c r="E32">
-        <f>D32-(D32*0.55)</f>
+        <f t="shared" si="0"/>
         <v>7.4492549999999991</v>
       </c>
       <c r="F32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G32">
         <v>3</v>
       </c>
-      <c r="H32" t="s">
-        <v>10</v>
+      <c r="H32">
+        <v>1</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>86</v>
+        <v>177</v>
       </c>
       <c r="K32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(31, '0000000000031', 'LEITE CONDENSADO S.LOURENCO 210G', 7.449255, 16.5539, 3, 'UN', 1, '2022-03-17', '2022-03-17', 1)</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33">
         <v>26.664000000000001</v>
       </c>
       <c r="E33">
-        <f>D33-(D33*0.55)</f>
+        <f t="shared" si="0"/>
         <v>11.998799999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G33">
         <v>5</v>
       </c>
-      <c r="H33" t="s">
-        <v>10</v>
+      <c r="H33">
+        <v>1</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="J33" s="5" t="s">
-        <v>86</v>
+        <v>178</v>
       </c>
       <c r="K33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(32, '0000000000032', 'LEITE CONDENSADO S.LOURENCO 335G', 11.9988, 26.664, 5, 'UN', 1, '2022-03-18', '2022-03-18', 1)</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34">
         <v>11.7766</v>
       </c>
       <c r="E34">
-        <f>D34-(D34*0.55)</f>
+        <f t="shared" si="0"/>
         <v>5.2994699999999995</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G34">
         <v>6</v>
       </c>
-      <c r="H34" t="s">
-        <v>10</v>
+      <c r="H34">
+        <v>1</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="K34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(33, '0000000000033', 'LEITE CONDENSADO S.LOURENCO S/LACT 380G', 5.29947, 11.7766, 6, 'UN', 1, '2022-03-19', '2022-03-19', 1)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D35" s="1"/>
     </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="5"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="5"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="5"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="5"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="5"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="5"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="5"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="5"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="5"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="5"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="5"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="5"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="5"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="5"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="5"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="5"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="5"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="5"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="5"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="5"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="5"/>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="5"/>
+    </row>
   </sheetData>
+  <sortState ref="B40:C72">
+    <sortCondition ref="C39"/>
+  </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2191,11 +2513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0B89C9-3387-4C9E-8B21-49BFEF44E7E5}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2205,74 +2527,90 @@
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>88</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D2" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="E2" t="str">
+        <f>"INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;")"</f>
+        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (1, 'APIARIOS MACKILANI LTDA', '10.340.623/0001-67', 7)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>89</v>
+      <c r="B3" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D3" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E5" si="0">"INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;")"</f>
+        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (2, 'SOARES E TECLES COM. REP. LTDA', '67.653.454/0001-32', 8)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>90</v>
+      <c r="B4" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D4" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (3, 'DISTRIBUIDORA MINEIRA DE DOCES LTDA', '60.888.582/0001-16', 9)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>91</v>
+      <c r="B5" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D5" s="3">
         <v>10</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (4, 'KAZJEL COM.REP.LTDA', '52.357.810/0001-01', 10)</v>
       </c>
     </row>
   </sheetData>
@@ -2281,16 +2619,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EFDD4D-4457-45D5-8AEE-C117D78E77F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2298,7 +2637,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2306,7 +2645,11 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C2" t="str">
+        <f>"INSERT INTO Categoria(CategoriaId, Nome) VALUES ("&amp;A2&amp;", "&amp;B2&amp;" )"</f>
+        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (1, 'DOCES/PASTAS' )</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,7 +2657,11 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C5" si="0">"INSERT INTO Categoria(CategoriaId, Nome) VALUES ("&amp;A3&amp;", "&amp;B3&amp;" )"</f>
+        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (2, 'SUPLEMENTO CAPSULA' )</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2322,7 +2669,11 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (3, 'SUPLEMENTO EM PÓ' )</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2330,7 +2681,11 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (4, 'OUTROS ALIMENTOS' )</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2345,23 +2700,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58E5BF0-3C77-43AF-80B1-EDA21D5CF829}">
-  <dimension ref="A1:F7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -2369,136 +2724,160 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>"INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;")"</f>
+        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(1, 'Leandro Nelson Carlos da Costa', '542.737.276-84', '(34) 99845-8473', 'leandronelsoncarlosdacosta@mail.com', 1)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G7" si="0">"INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;")"</f>
+        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(2, 'Rosa Yasmin Daiane', '026.626.186-80', '(34) 98715-9676', 'rosayasmindaiane@outlook.com', 2)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(3, 'Nina Jennifer Isabel', '683.112.266-36', '(34) 99813-3514', 'ninajenniferisabel@outlook.com', 3)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(4, 'Thomas Yago da Mota', '741.781.786-60', '(34) 98736-9088', 'thomasyagodamota@yahoo.com', 4)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(5, 'Danilo Severino Nathan Ribeiro', '516.413.856-50', '(34) 99779-7817', 'daniloseverinonathanribeiro@gmail.com', 5)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F7">
         <v>6</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(6, 'Calebe Anderson Peixoto', '846.236.776-05', '(34) 99889-9582', 'calebeandersonpeixoto@hotmail.com', 6)</v>
       </c>
     </row>
   </sheetData>
@@ -2507,11 +2886,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB24E19D-776A-455D-AFFE-6E4686594A72}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,257 +2899,297 @@
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G2" s="1">
         <v>759</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>"INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;")"</f>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (1, '38400-670', 'Rua José Rezende dos Santos', 'Brasil', 'Uberlândia', 'MG', 759)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G3" s="1">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H11" si="0">"INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;")"</f>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (2, '38421-046', 'Rua do Sai-Azul', 'Loteamento Residencial Pequis', 'Uberlândia', 'MG', 356)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G4" s="1">
         <v>358</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (3, '38421-643', 'Rua Odécio dos Santos', 'Residencial Lago Azul', 'Uberlândia', 'MG', 358)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G5" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (4, '38433-018', 'Rua Quatro', 'Vila Marielza', 'Uberlândia', 'MG', 999)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G6" s="1">
         <v>657</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (5, '38400-708', 'Avenida Afonso Pena', 'Nossa Senhora Aparecida', 'Uberlândia', 'MG', 657)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G7" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (6, '38400-329', 'Avenida Getúlio Vargas', 'Daniel Fonseca', 'Uberlândia', 'MG', 60)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
-      </c>
-      <c r="F8" t="s">
-        <v>101</v>
+        <v>124</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G8">
         <v>253</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (7, '32240-351', 'Beco Caramuru', 'Bandeirantes', 'Contagem', 'MG', 253)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="E9" t="s">
-        <v>156</v>
-      </c>
-      <c r="F9" t="s">
-        <v>101</v>
+        <v>128</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G9">
         <v>272</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (8, '35302-660', 'Rua Marcelo Moreira Rezende de Araújo', 'Rafael José de Lima', 'Caratinga', 'MG', 272)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F10" t="s">
-        <v>101</v>
+        <v>132</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G10">
         <v>918</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (9, '38071-306', 'Avenida Doutor Milton Campos', 'Vila Arquelau', 'Uberaba', 'MG', 918)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="E11" t="s">
-        <v>164</v>
-      </c>
-      <c r="F11" t="s">
-        <v>101</v>
+        <v>136</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="G11">
         <v>654</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (10, '31540-474', 'Beco B', 'Jardim Leblon', 'Belo Horizonte', 'MG', 654)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Criado controller para testar as funções de CRUD da classe produto
</commit_message>
<xml_diff>
--- a/Database/DadosIniciais.xlsx
+++ b/Database/DadosIniciais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUTOS" sheetId="1" r:id="rId1"/>
@@ -983,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,8 +1073,8 @@
         <v>1</v>
       </c>
       <c r="L2" t="str">
-        <f>"INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;E2&amp;", "&amp;D2&amp;", "&amp;G2&amp;", "&amp;F2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;")"</f>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(1, '0000000000001', 'ABSOLUT PASTA AMENDOIM BEIJINHO 1KG', 19.948005, 44.3289, 9, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+        <f>"INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;E2&amp;", "&amp;D2&amp;", "&amp;G2&amp;", "&amp;F2&amp;", "&amp;H2&amp;", "&amp;I2&amp;", "&amp;J2&amp;", "&amp;K2&amp;")"</f>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(1, '0000000000001', 'ABSOLUT PASTA AMENDOIM BEIJINHO 1KG', 19.948005, 44.3289, 9, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1113,8 +1113,8 @@
         <v>1</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:L34" si="1">"INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;E3&amp;", "&amp;D3&amp;", "&amp;G3&amp;", "&amp;F3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;")"</f>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(2, '0000000000002', 'ABSOLUT PASTA AMENDOIM BEIJINHO 500G', 14.948505, 33.2189, 8, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+        <f t="shared" ref="L3:L34" si="1">"INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;E3&amp;", "&amp;D3&amp;", "&amp;G3&amp;", "&amp;F3&amp;", "&amp;H3&amp;", "&amp;I3&amp;", "&amp;J3&amp;", "&amp;K3&amp;")"</f>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(2, '0000000000002', 'ABSOLUT PASTA AMENDOIM BEIJINHO 500G', 14.948505, 33.2189, 8, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="L4" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(3, '0000000000003', 'ABSOLUT PASTA AMENDOIM BROWNIE 1KG', 19.948005, 44.3289, 7, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(3, '0000000000003', 'ABSOLUT PASTA AMENDOIM BROWNIE 1KG', 19.948005, 44.3289, 7, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="L5" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(4, '0000000000004', 'ABSOLUT PASTA AMENDOIM BROWNIE 500G', 14.948505, 33.2189, 4, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(4, '0000000000004', 'ABSOLUT PASTA AMENDOIM BROWNIE 500G', 14.948505, 33.2189, 4, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1234,7 +1234,7 @@
       </c>
       <c r="L6" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(5, '0000000000005', 'ACAI BANANA ECO FLASH 200G', 3.8746125, 8.61025, 5, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(5, '0000000000005', 'ACAI BANANA ECO FLASH 200G', 3.8746125, 8.61025, 5, 'UN', 1, '2022-03-01', '2022-03-01', 1)</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="L7" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(6, '0000000000006', 'ACAI DESIDRATADO TIARAJU 150G', 12.448755, 27.6639, 6, 'UN', 1, '2022-03-02', '2022-03-02', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(6, '0000000000006', 'ACAI DESIDRATADO TIARAJU 150G', 12.448755, 27.6639, 6, 'UN', 1, '2022-03-02', '2022-03-02', 1)</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1314,7 +1314,7 @@
       </c>
       <c r="L8" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(7, '0000000000007', 'ACAI ECO FLESH GUARANA 1000G', 12.948705, 28.7749, 4, 'UN', 1, '2022-03-02', '2022-03-02', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(7, '0000000000007', 'ACAI ECO FLESH GUARANA 1000G', 12.948705, 28.7749, 4, 'UN', 1, '2022-03-02', '2022-03-02', 1)</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="L9" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(8, '0000000000008', 'ADOCANTE ABSOLUT 100% ESTEVIA 150G', 17.448255, 38.7739, 5, 'UN', 1, '2022-03-03', '2022-03-03', 4)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(8, '0000000000008', 'ADOCANTE ABSOLUT 100% ESTEVIA 150G', 17.448255, 38.7739, 5, 'UN', 1, '2022-03-03', '2022-03-03', 4)</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(9, '0000000000009', 'ADOCANTE ABSOLUT 100% XYLITOL 300G', 19.948005, 44.3289, 8, 'UN', 1, '2022-03-03', '2022-03-03', 4)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(9, '0000000000009', 'ADOCANTE ABSOLUT 100% XYLITOL 300G', 19.948005, 44.3289, 8, 'UN', 1, '2022-03-03', '2022-03-03', 4)</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="L11" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(10, '0000000000010', 'ADOCANTE AIROM TAUMATINA 100 ML', 8.19918, 18.2204, 9, 'UN', 1, '2022-03-04', '2022-03-04', 4)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(10, '0000000000010', 'ADOCANTE AIROM TAUMATINA 100 ML', 8.19918, 18.2204, 9, 'UN', 1, '2022-03-04', '2022-03-04', 4)</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="L12" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(11, '0000000000011', 'ALBUMINA MILLENNIUM BAUNILHA 500G', 26.947305, 59.8829, 6, 'UN', 1, '2022-03-04', '2022-03-04', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(11, '0000000000011', 'ALBUMINA MILLENNIUM BAUNILHA 500G', 26.947305, 59.8829, 6, 'UN', 1, '2022-03-04', '2022-03-04', 2)</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="L13" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(12, '0000000000012', 'ALBUMINA MILLENNIUM CHOCOLATE 500G', 26.947305, 59.8829, 8, 'UN', 1, '2022-03-04', '2022-03-04', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(12, '0000000000012', 'ALBUMINA MILLENNIUM CHOCOLATE 500G', 26.947305, 59.8829, 8, 'UN', 1, '2022-03-04', '2022-03-04', 2)</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="L14" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(13, '0000000000013', 'ALBUMINA MILLENNIUM MOR.BANANA.500G', 26.947305, 59.8829, 5, 'UN', 1, '2022-03-05', '2022-03-05', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(13, '0000000000013', 'ALBUMINA MILLENNIUM MOR.BANANA.500G', 26.947305, 59.8829, 5, 'UN', 1, '2022-03-05', '2022-03-05', 2)</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="L15" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(14, '0000000000014', 'BANANINHA HUE 117G', 5.749425, 12.7765, 5, 'UN', 1, '2022-03-06', '2022-03-06', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(14, '0000000000014', 'BANANINHA HUE 117G', 5.749425, 12.7765, 5, 'UN', 1, '2022-03-06', '2022-03-06', 2)</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="L16" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(15, '0000000000015', 'BANANINHA NUTRYLLACK 28G', 6.449355, 14.3319, 7, 'UN', 1, '2022-03-06', '2022-03-06', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(15, '0000000000015', 'BANANINHA NUTRYLLACK 28G', 6.449355, 14.3319, 7, 'UN', 1, '2022-03-06', '2022-03-06', 2)</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="L17" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(16, '0000000000016', 'BANANINHA PASSA TIPIKUS 1 KG', 13.948605, 30.9969, 4, 'UN', 1, '2022-03-08', '2022-03-08', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(16, '0000000000016', 'BANANINHA PASSA TIPIKUS 1 KG', 13.948605, 30.9969, 4, 'UN', 1, '2022-03-08', '2022-03-08', 2)</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="L18" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(17, '0000000000017', 'BCAA PLUS PROBIOTICA 120 CAP', 51.944805, 115.4329, 9, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(17, '0000000000017', 'BCAA PLUS PROBIOTICA 120 CAP', 51.944805, 115.4329, 9, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1754,7 +1754,7 @@
       </c>
       <c r="L19" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(18, '0000000000018', 'BCAA PRO PROBIOTICA 120 CAP', 37.8212175, 84.04715, 5, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(18, '0000000000018', 'BCAA PRO PROBIOTICA 120 CAP', 37.8212175, 84.04715, 5, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="L20" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(19, '0000000000019', 'BCAA PRO PROBIOTICA 60 CAPS', 17.448255, 38.7739, 3, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(19, '0000000000019', 'BCAA PRO PROBIOTICA 60 CAPS', 17.448255, 38.7739, 3, 'UN', 1, '2022-03-09', '2022-03-09', 3)</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="L21" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(20, '0000000000020', 'BCAA PROBIOTICA BLACK NATURAL 300G', 87.49125, 194.425, 8, 'UN', 1, '2022-03-09', '2022-03-09', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(20, '0000000000020', 'BCAA PROBIOTICA BLACK NATURAL 300G', 87.49125, 194.425, 8, 'UN', 1, '2022-03-09', '2022-03-09', 2)</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="L22" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(21, '0000000000021', 'CREATINA INTEGRAL 100G', 18.49815, 41.107, 9, 'UN', 1, '2022-03-10', '2022-03-10', 2)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(21, '0000000000021', 'CREATINA INTEGRAL 100G', 18.49815, 41.107, 9, 'UN', 1, '2022-03-10', '2022-03-10', 2)</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="L23" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(22, '0000000000022', 'CREATINA INTEGRAL 120 CAPS', 32.446755, 72.1039, 9, 'UN', 1, '2022-03-10', '2022-03-10', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(22, '0000000000022', 'CREATINA INTEGRAL 120 CAPS', 32.446755, 72.1039, 9, 'UN', 1, '2022-03-10', '2022-03-10', 3)</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="L24" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(23, '0000000000023', 'CREATINA INTEGRAL 120 CPS', 41.745825, 92.7685, 3, 'UN', 1, '2022-03-11', '2022-03-11', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(23, '0000000000023', 'CREATINA INTEGRAL 120 CPS', 41.745825, 92.7685, 3, 'UN', 1, '2022-03-11', '2022-03-11', 3)</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(24, '0000000000024', 'CRISTAIS GENGIBRE ARDRAK ANIS 22G', 5.6744325, 12.60985, 5, 'UN', 1, '2022-03-12', '2022-03-12', 4)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(24, '0000000000024', 'CRISTAIS GENGIBRE ARDRAK ANIS 22G', 5.6744325, 12.60985, 5, 'UN', 1, '2022-03-12', '2022-03-12', 4)</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
       </c>
       <c r="L26" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(25, '0000000000025', 'CRISTAIS GENGIBRE ARDRAK CANELA 22G', 5.6744325, 12.60985, 5, 'UN', 1, '2022-03-13', '2022-03-13', 4)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(25, '0000000000025', 'CRISTAIS GENGIBRE ARDRAK CANELA 22G', 5.6744325, 12.60985, 5, 'UN', 1, '2022-03-13', '2022-03-13', 4)</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="L27" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(26, '0000000000026', 'CRISTAIS GENGIBRE ARDRAK FRU.CITRICAS 22G', 5.6744325, 12.60985, 7, 'UN', 1, '2022-03-14', '2022-03-14', 4)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(26, '0000000000026', 'CRISTAIS GENGIBRE ARDRAK FRU.CITRICAS 22G', 5.6744325, 12.60985, 7, 'UN', 1, '2022-03-14', '2022-03-14', 4)</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="L28" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(27, '0000000000027', 'ISO 100 WHEY DYMATIZE BAUNILHA 726G', 172.48275, 383.295, 7, 'UN', 1, '2022-03-14', '2022-03-14', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(27, '0000000000027', 'ISO 100 WHEY DYMATIZE BAUNILHA 726G', 172.48275, 383.295, 7, 'UN', 1, '2022-03-14', '2022-03-14', 3)</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="L29" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(28, '0000000000028', 'ISO 100 WHEY DYMATIZE BOLO ANIVERSARIO 726G', 172.48275, 383.295, 7, 'UN', 1, '2022-03-14', '2022-03-14', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(28, '0000000000028', 'ISO 100 WHEY DYMATIZE BOLO ANIVERSARIO 726G', 172.48275, 383.295, 7, 'UN', 1, '2022-03-14', '2022-03-14', 3)</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="L30" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(29, '0000000000029', 'ISO 100 WHEY DYMATIZE BROWNIE 893G', 179.48205, 398.849, 4, 'UN', 1, '2022-03-15', '2022-03-15', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(29, '0000000000029', 'ISO 100 WHEY DYMATIZE BROWNIE 893G', 179.48205, 398.849, 4, 'UN', 1, '2022-03-15', '2022-03-15', 3)</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="L31" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(30, '0000000000030', 'ISO 100 WHEY DYMATIZE CAKE 893G', 179.48205, 398.849, 3, 'UN', 1, '2022-03-16', '2022-03-16', 3)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(30, '0000000000030', 'ISO 100 WHEY DYMATIZE CAKE 893G', 179.48205, 398.849, 3, 'UN', 1, '2022-03-16', '2022-03-16', 3)</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="L32" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(31, '0000000000031', 'LEITE CONDENSADO S.LOURENCO 210G', 7.449255, 16.5539, 3, 'UN', 1, '2022-03-17', '2022-03-17', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(31, '0000000000031', 'LEITE CONDENSADO S.LOURENCO 210G', 7.449255, 16.5539, 3, 'UN', 1, '2022-03-17', '2022-03-17', 1)</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="L33" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(32, '0000000000032', 'LEITE CONDENSADO S.LOURENCO 335G', 11.9988, 26.664, 5, 'UN', 1, '2022-03-18', '2022-03-18', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(32, '0000000000032', 'LEITE CONDENSADO S.LOURENCO 335G', 11.9988, 26.664, 5, 'UN', 1, '2022-03-18', '2022-03-18', 1)</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="L34" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO Produto(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(33, '0000000000033', 'LEITE CONDENSADO S.LOURENCO S/LACT 380G', 5.29947, 11.7766, 6, 'UN', 1, '2022-03-19', '2022-03-19', 1)</v>
+        <v>INSERT INTO Produtos(ProdutoId,CodBarras,Descricao,PrecoCusto,PrecoVenda,Estoque,UniMedida,Ativo,DataCadastro,UltimaAlteracao,CategoriaId) VALUES(33, '0000000000033', 'LEITE CONDENSADO S.LOURENCO S/LACT 380G', 5.29947, 11.7766, 6, 'UN', 1, '2022-03-19', '2022-03-19', 1)</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -2555,8 +2555,8 @@
         <v>7</v>
       </c>
       <c r="E2" t="str">
-        <f>"INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;")"</f>
-        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (1, 'APIARIOS MACKILANI LTDA', '10.340.623/0001-67', 7)</v>
+        <f>"INSERT INTO Fornecedores(FornecedorId, Nome, CNPJ, EnderecoId) VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;")"</f>
+        <v>INSERT INTO Fornecedores(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (1, 'APIARIOS MACKILANI LTDA', '10.340.623/0001-67', 7)</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2573,8 +2573,8 @@
         <v>8</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E5" si="0">"INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;")"</f>
-        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (2, 'SOARES E TECLES COM. REP. LTDA', '67.653.454/0001-32', 8)</v>
+        <f t="shared" ref="E3:E5" si="0">"INSERT INTO Fornecedores(FornecedorId, Nome, CNPJ, EnderecoId) VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;")"</f>
+        <v>INSERT INTO Fornecedores(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (2, 'SOARES E TECLES COM. REP. LTDA', '67.653.454/0001-32', 8)</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (3, 'DISTRIBUIDORA MINEIRA DE DOCES LTDA', '60.888.582/0001-16', 9)</v>
+        <v>INSERT INTO Fornecedores(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (3, 'DISTRIBUIDORA MINEIRA DE DOCES LTDA', '60.888.582/0001-16', 9)</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Fornecedor(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (4, 'KAZJEL COM.REP.LTDA', '52.357.810/0001-01', 10)</v>
+        <v>INSERT INTO Fornecedores(FornecedorId, Nome, CNPJ, EnderecoId) VALUES (4, 'KAZJEL COM.REP.LTDA', '52.357.810/0001-01', 10)</v>
       </c>
     </row>
   </sheetData>
@@ -2622,7 +2622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
@@ -2648,8 +2648,8 @@
         <v>14</v>
       </c>
       <c r="C2" t="str">
-        <f>"INSERT INTO Categoria(CategoriaId, Nome) VALUES ("&amp;A2&amp;", "&amp;B2&amp;" )"</f>
-        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (1, 'DOCES/PASTAS' )</v>
+        <f>"INSERT INTO Categorias(CategoriaId, Nome) VALUES ("&amp;A2&amp;", "&amp;B2&amp;" )"</f>
+        <v>INSERT INTO Categorias(CategoriaId, Nome) VALUES (1, 'DOCES/PASTAS' )</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2660,8 +2660,8 @@
         <v>15</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C5" si="0">"INSERT INTO Categoria(CategoriaId, Nome) VALUES ("&amp;A3&amp;", "&amp;B3&amp;" )"</f>
-        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (2, 'SUPLEMENTO CAPSULA' )</v>
+        <f t="shared" ref="C3:C5" si="0">"INSERT INTO Categorias(CategoriaId, Nome) VALUES ("&amp;A3&amp;", "&amp;B3&amp;" )"</f>
+        <v>INSERT INTO Categorias(CategoriaId, Nome) VALUES (2, 'SUPLEMENTO CAPSULA' )</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (3, 'SUPLEMENTO EM PÓ' )</v>
+        <v>INSERT INTO Categorias(CategoriaId, Nome) VALUES (3, 'SUPLEMENTO EM PÓ' )</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Categoria(CategoriaId, Nome) VALUES (4, 'OUTROS ALIMENTOS' )</v>
+        <v>INSERT INTO Categorias(CategoriaId, Nome) VALUES (4, 'OUTROS ALIMENTOS' )</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2756,8 +2756,8 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <f>"INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;")"</f>
-        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(1, 'Leandro Nelson Carlos da Costa', '542.737.276-84', '(34) 99845-8473', 'leandronelsoncarlosdacosta@mail.com', 1)</v>
+        <f>"INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;")"</f>
+        <v>INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(1, 'Leandro Nelson Carlos da Costa', '542.737.276-84', '(34) 99845-8473', 'leandronelsoncarlosdacosta@mail.com', 1)</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2780,8 +2780,8 @@
         <v>2</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G7" si="0">"INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;")"</f>
-        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(2, 'Rosa Yasmin Daiane', '026.626.186-80', '(34) 98715-9676', 'rosayasmindaiane@outlook.com', 2)</v>
+        <f t="shared" ref="G3:G7" si="0">"INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;")"</f>
+        <v>INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(2, 'Rosa Yasmin Daiane', '026.626.186-80', '(34) 98715-9676', 'rosayasmindaiane@outlook.com', 2)</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(3, 'Nina Jennifer Isabel', '683.112.266-36', '(34) 99813-3514', 'ninajenniferisabel@outlook.com', 3)</v>
+        <v>INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(3, 'Nina Jennifer Isabel', '683.112.266-36', '(34) 99813-3514', 'ninajenniferisabel@outlook.com', 3)</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2829,7 +2829,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(4, 'Thomas Yago da Mota', '741.781.786-60', '(34) 98736-9088', 'thomasyagodamota@yahoo.com', 4)</v>
+        <v>INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(4, 'Thomas Yago da Mota', '741.781.786-60', '(34) 98736-9088', 'thomasyagodamota@yahoo.com', 4)</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(5, 'Danilo Severino Nathan Ribeiro', '516.413.856-50', '(34) 99779-7817', 'daniloseverinonathanribeiro@gmail.com', 5)</v>
+        <v>INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(5, 'Danilo Severino Nathan Ribeiro', '516.413.856-50', '(34) 99779-7817', 'daniloseverinonathanribeiro@gmail.com', 5)</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Solicitante(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(6, 'Calebe Anderson Peixoto', '846.236.776-05', '(34) 99889-9582', 'calebeandersonpeixoto@hotmail.com', 6)</v>
+        <v>INSERT INTO Solicitantes(SolicitanteId, Nome, CPF, Telefone, Email, EnderecoId) VALUES(6, 'Calebe Anderson Peixoto', '846.236.776-05', '(34) 99889-9582', 'calebeandersonpeixoto@hotmail.com', 6)</v>
       </c>
     </row>
   </sheetData>
@@ -2945,8 +2945,8 @@
         <v>759</v>
       </c>
       <c r="H2" t="str">
-        <f>"INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;")"</f>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (1, '38400-670', 'Rua José Rezende dos Santos', 'Brasil', 'Uberlândia', 'MG', 759)</v>
+        <f>"INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES ("&amp;A2&amp;", "&amp;B2&amp;", "&amp;C2&amp;", "&amp;D2&amp;", "&amp;E2&amp;", "&amp;F2&amp;", "&amp;G2&amp;")"</f>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (1, '38400-670', 'Rua José Rezende dos Santos', 'Brasil', 'Uberlândia', 'MG', 759)</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2972,8 +2972,8 @@
         <v>356</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H11" si="0">"INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;")"</f>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (2, '38421-046', 'Rua do Sai-Azul', 'Loteamento Residencial Pequis', 'Uberlândia', 'MG', 356)</v>
+        <f t="shared" ref="H3:H11" si="0">"INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES ("&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;", "&amp;D3&amp;", "&amp;E3&amp;", "&amp;F3&amp;", "&amp;G3&amp;")"</f>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (2, '38421-046', 'Rua do Sai-Azul', 'Loteamento Residencial Pequis', 'Uberlândia', 'MG', 356)</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (3, '38421-643', 'Rua Odécio dos Santos', 'Residencial Lago Azul', 'Uberlândia', 'MG', 358)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (3, '38421-643', 'Rua Odécio dos Santos', 'Residencial Lago Azul', 'Uberlândia', 'MG', 358)</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3027,7 +3027,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (4, '38433-018', 'Rua Quatro', 'Vila Marielza', 'Uberlândia', 'MG', 999)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (4, '38433-018', 'Rua Quatro', 'Vila Marielza', 'Uberlândia', 'MG', 999)</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -3054,7 +3054,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (5, '38400-708', 'Avenida Afonso Pena', 'Nossa Senhora Aparecida', 'Uberlândia', 'MG', 657)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (5, '38400-708', 'Avenida Afonso Pena', 'Nossa Senhora Aparecida', 'Uberlândia', 'MG', 657)</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (6, '38400-329', 'Avenida Getúlio Vargas', 'Daniel Fonseca', 'Uberlândia', 'MG', 60)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (6, '38400-329', 'Avenida Getúlio Vargas', 'Daniel Fonseca', 'Uberlândia', 'MG', 60)</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (7, '32240-351', 'Beco Caramuru', 'Bandeirantes', 'Contagem', 'MG', 253)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (7, '32240-351', 'Beco Caramuru', 'Bandeirantes', 'Contagem', 'MG', 253)</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (8, '35302-660', 'Rua Marcelo Moreira Rezende de Araújo', 'Rafael José de Lima', 'Caratinga', 'MG', 272)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (8, '35302-660', 'Rua Marcelo Moreira Rezende de Araújo', 'Rafael José de Lima', 'Caratinga', 'MG', 272)</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (9, '38071-306', 'Avenida Doutor Milton Campos', 'Vila Arquelau', 'Uberaba', 'MG', 918)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (9, '38071-306', 'Avenida Doutor Milton Campos', 'Vila Arquelau', 'Uberaba', 'MG', 918)</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO Endereco (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (10, '31540-474', 'Beco B', 'Jardim Leblon', 'Belo Horizonte', 'MG', 654)</v>
+        <v>INSERT INTO Enderecos (EnderecoId, Cep, Logradouro, Bairro, Cidade, Uf, Numero) VALUES (10, '31540-474', 'Beco B', 'Jardim Leblon', 'Belo Horizonte', 'MG', 654)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>